<commit_message>
Changed control of asset name from text box to combo box
</commit_message>
<xml_diff>
--- a/Documents/Laboratory Asset-Inventory_JIga.xlsx
+++ b/Documents/Laboratory Asset-Inventory_JIga.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yura\Documents\Projects\PNGIMR_IS\PNGIMR_IS\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="11355" windowHeight="10230"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <definedName name="vertex42_id" hidden="1">"asset-tracking-template.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Asset Tracking Template"</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2032,17 +2037,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="169" formatCode="_-[$PGK]\ * #,##0.00_-;\-[$PGK]\ * #,##0.00_-;_-[$PGK]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="m/d;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="167" formatCode="_-[$PGK]\ * #,##0.00_-;\-[$PGK]\ * #,##0.00_-;_-[$PGK]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="58">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2705,7 +2710,7 @@
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2744,7 +2749,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2767,7 +2772,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2781,7 +2786,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2791,7 +2796,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="10" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="10" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2803,7 +2808,7 @@
     <xf numFmtId="0" fontId="31" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2826,7 +2831,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="24" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2877,10 +2882,10 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="47" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="47" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="47" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2907,7 +2912,7 @@
     <xf numFmtId="14" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2922,13 +2927,13 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="53" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="53" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="53" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="25" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2943,25 +2948,25 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="55" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="55" fillId="0" borderId="7" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="53" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="53" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="47" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="47" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="53" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="53" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2973,10 +2978,10 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="56" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="56" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="56" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="56" fillId="0" borderId="7" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3048,7 +3053,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3083,7 +3088,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3118,7 +3123,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3153,7 +3158,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3188,7 +3193,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3223,7 +3228,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3258,7 +3263,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3292,7 +3297,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3327,7 +3332,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3362,7 +3367,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3397,7 +3402,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3432,7 +3437,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3473,7 +3478,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3497,7 +3502,7 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -3517,7 +3522,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3544,7 +3549,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3572,8 +3577,8 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="m/d;@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <numFmt numFmtId="168" formatCode="m/d;@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -3599,7 +3604,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3631,8 +3636,8 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3666,7 +3671,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3700,8 +3705,8 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3735,7 +3740,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3769,7 +3774,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3803,7 +3808,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3837,7 +3842,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3871,7 +3876,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3905,7 +3910,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3939,7 +3944,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -3973,7 +3978,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4007,7 +4012,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4041,7 +4046,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4075,7 +4080,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4109,7 +4114,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4143,7 +4148,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4177,7 +4182,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4211,7 +4216,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4245,7 +4250,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4279,7 +4284,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="55"/>
@@ -4320,7 +4325,7 @@
         <name val="Trebuchet MS"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4344,7 +4349,7 @@
           <bgColor indexed="23"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
@@ -4430,13 +4435,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:X207" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
-  <autoFilter ref="A8:X207">
-    <filterColumn colId="15"/>
-    <filterColumn colId="16"/>
-    <filterColumn colId="21"/>
-    <filterColumn colId="22"/>
-    <filterColumn colId="23"/>
-  </autoFilter>
+  <autoFilter ref="A8:X207"/>
   <tableColumns count="24">
     <tableColumn id="1" name="Name" dataDxfId="38"/>
     <tableColumn id="13" name="Brand" dataDxfId="37"/>
@@ -4457,7 +4456,7 @@
     <tableColumn id="15" name="Confirmity (Acc.Asset Registry)" dataDxfId="22"/>
     <tableColumn id="7" name="Date" dataDxfId="21"/>
     <tableColumn id="8" name="Supplier" dataDxfId="20"/>
-    <tableColumn id="9" name="Warranty&#10;Expiration" dataDxfId="19"/>
+    <tableColumn id="9" name="Warranty_x000a_Expiration" dataDxfId="19"/>
     <tableColumn id="10" name="Price" dataDxfId="18" dataCellStyle="Currency"/>
     <tableColumn id="17" name="Decontaminated" dataDxfId="17"/>
     <tableColumn id="18" name="Disposed using Town general waste removal." dataDxfId="16"/>
@@ -4472,10 +4471,10 @@
   <tableColumns count="12">
     <tableColumn id="1" name="Supplier Name" dataDxfId="11"/>
     <tableColumn id="2" name="Product" dataDxfId="10"/>
-    <tableColumn id="3" name="Product Link&#10;(website)" dataDxfId="9"/>
+    <tableColumn id="3" name="Product Link_x000a_(website)" dataDxfId="9"/>
     <tableColumn id="4" name="Description" dataDxfId="8"/>
     <tableColumn id="5" name="Price" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Lead Time&#10;(days)" dataDxfId="6"/>
+    <tableColumn id="6" name="Lead Time_x000a_(days)" dataDxfId="6"/>
     <tableColumn id="7" name="Contact Name" dataDxfId="5"/>
     <tableColumn id="8" name="Email" dataDxfId="4"/>
     <tableColumn id="9" name="Phone #" dataDxfId="3"/>
@@ -4713,18 +4712,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X207"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A135" sqref="A135:XFD135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
@@ -4752,7 +4751,7 @@
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30">
+    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
@@ -4762,12 +4761,12 @@
       <c r="T1" s="3"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="12.75" customHeight="1">
+    <row r="2" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="20.25">
+    <row r="3" spans="1:24" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -4775,16 +4774,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="16.5">
+    <row r="4" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="11">
         <f ca="1">TODAY()</f>
-        <v>44074</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="18.75">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>475</v>
       </c>
@@ -4792,8 +4791,8 @@
         <v>476</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1"/>
-    <row r="7" spans="1:24" ht="16.5">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="48" customHeight="1">
+    <row r="8" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>0</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="8" customFormat="1">
+    <row r="9" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -4959,7 +4958,7 @@
       <c r="W9" s="91"/>
       <c r="X9" s="91"/>
     </row>
-    <row r="10" spans="1:24" s="8" customFormat="1">
+    <row r="10" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -5013,7 +5012,7 @@
       <c r="W10" s="91"/>
       <c r="X10" s="91"/>
     </row>
-    <row r="11" spans="1:24" s="8" customFormat="1">
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -5061,7 +5060,7 @@
       <c r="W11" s="91"/>
       <c r="X11" s="91"/>
     </row>
-    <row r="12" spans="1:24" s="8" customFormat="1">
+    <row r="12" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -5111,7 +5110,7 @@
       <c r="W12" s="91"/>
       <c r="X12" s="91"/>
     </row>
-    <row r="13" spans="1:24" s="8" customFormat="1">
+    <row r="13" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -5157,7 +5156,7 @@
       <c r="W13" s="91"/>
       <c r="X13" s="91"/>
     </row>
-    <row r="14" spans="1:24" s="8" customFormat="1">
+    <row r="14" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -5203,7 +5202,7 @@
       <c r="W14" s="91"/>
       <c r="X14" s="91"/>
     </row>
-    <row r="15" spans="1:24" s="8" customFormat="1">
+    <row r="15" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -5245,7 +5244,7 @@
       <c r="W15" s="91"/>
       <c r="X15" s="91"/>
     </row>
-    <row r="16" spans="1:24" s="8" customFormat="1">
+    <row r="16" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>54</v>
       </c>
@@ -5289,7 +5288,7 @@
       <c r="W16" s="91"/>
       <c r="X16" s="91"/>
     </row>
-    <row r="17" spans="1:24" s="8" customFormat="1">
+    <row r="17" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>54</v>
       </c>
@@ -5333,7 +5332,7 @@
       <c r="W17" s="91"/>
       <c r="X17" s="91"/>
     </row>
-    <row r="18" spans="1:24" s="8" customFormat="1">
+    <row r="18" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
@@ -5387,7 +5386,7 @@
       <c r="W18" s="91"/>
       <c r="X18" s="91"/>
     </row>
-    <row r="19" spans="1:24" s="8" customFormat="1" ht="30">
+    <row r="19" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>108</v>
       </c>
@@ -5439,7 +5438,7 @@
       <c r="W19" s="91"/>
       <c r="X19" s="91"/>
     </row>
-    <row r="20" spans="1:24" s="8" customFormat="1">
+    <row r="20" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
@@ -5491,7 +5490,7 @@
       <c r="W20" s="91"/>
       <c r="X20" s="91"/>
     </row>
-    <row r="21" spans="1:24" s="8" customFormat="1">
+    <row r="21" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -5541,7 +5540,7 @@
       <c r="W21" s="91"/>
       <c r="X21" s="91"/>
     </row>
-    <row r="22" spans="1:24" s="8" customFormat="1">
+    <row r="22" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -5589,7 +5588,7 @@
       <c r="W22" s="91"/>
       <c r="X22" s="91"/>
     </row>
-    <row r="23" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="23" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>57</v>
       </c>
@@ -5639,7 +5638,7 @@
       <c r="W23" s="91"/>
       <c r="X23" s="91"/>
     </row>
-    <row r="24" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="24" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>57</v>
       </c>
@@ -5691,7 +5690,7 @@
       <c r="W24" s="91"/>
       <c r="X24" s="91"/>
     </row>
-    <row r="25" spans="1:24" s="8" customFormat="1" ht="40.5">
+    <row r="25" spans="1:24" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>62</v>
       </c>
@@ -5743,7 +5742,7 @@
       <c r="W25" s="91"/>
       <c r="X25" s="91"/>
     </row>
-    <row r="26" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="26" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>69</v>
       </c>
@@ -5797,7 +5796,7 @@
       <c r="W26" s="91"/>
       <c r="X26" s="91"/>
     </row>
-    <row r="27" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="27" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>69</v>
       </c>
@@ -5849,7 +5848,7 @@
       <c r="W27" s="91"/>
       <c r="X27" s="91"/>
     </row>
-    <row r="28" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="28" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>69</v>
       </c>
@@ -5899,7 +5898,7 @@
       <c r="W28" s="91"/>
       <c r="X28" s="91"/>
     </row>
-    <row r="29" spans="1:24" s="8" customFormat="1">
+    <row r="29" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="73" t="s">
         <v>648</v>
       </c>
@@ -5945,7 +5944,7 @@
       <c r="W29" s="91"/>
       <c r="X29" s="91"/>
     </row>
-    <row r="30" spans="1:24" s="8" customFormat="1">
+    <row r="30" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>51</v>
       </c>
@@ -5995,7 +5994,7 @@
       <c r="W30" s="91"/>
       <c r="X30" s="91"/>
     </row>
-    <row r="31" spans="1:24" s="8" customFormat="1">
+    <row r="31" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -6047,7 +6046,7 @@
       <c r="W31" s="91"/>
       <c r="X31" s="91"/>
     </row>
-    <row r="32" spans="1:24" s="8" customFormat="1">
+    <row r="32" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>45</v>
       </c>
@@ -6099,7 +6098,7 @@
       <c r="W32" s="91"/>
       <c r="X32" s="91"/>
     </row>
-    <row r="33" spans="1:24" s="8" customFormat="1">
+    <row r="33" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>52</v>
       </c>
@@ -6149,7 +6148,7 @@
       <c r="W33" s="91"/>
       <c r="X33" s="91"/>
     </row>
-    <row r="34" spans="1:24" s="8" customFormat="1">
+    <row r="34" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>51</v>
       </c>
@@ -6197,7 +6196,7 @@
       <c r="W34" s="91"/>
       <c r="X34" s="91"/>
     </row>
-    <row r="35" spans="1:24" s="8" customFormat="1">
+    <row r="35" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>51</v>
       </c>
@@ -6247,7 +6246,7 @@
       <c r="W35" s="91"/>
       <c r="X35" s="91"/>
     </row>
-    <row r="36" spans="1:24" s="8" customFormat="1">
+    <row r="36" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>48</v>
       </c>
@@ -6297,7 +6296,7 @@
       <c r="W36" s="91"/>
       <c r="X36" s="91"/>
     </row>
-    <row r="37" spans="1:24" s="8" customFormat="1">
+    <row r="37" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -6345,7 +6344,7 @@
       <c r="W37" s="91"/>
       <c r="X37" s="91"/>
     </row>
-    <row r="38" spans="1:24" s="8" customFormat="1">
+    <row r="38" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>46</v>
       </c>
@@ -6393,7 +6392,7 @@
       <c r="W38" s="91"/>
       <c r="X38" s="91"/>
     </row>
-    <row r="39" spans="1:24" s="8" customFormat="1">
+    <row r="39" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>133</v>
       </c>
@@ -6441,7 +6440,7 @@
       <c r="W39" s="91"/>
       <c r="X39" s="91"/>
     </row>
-    <row r="40" spans="1:24" s="8" customFormat="1">
+    <row r="40" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>51</v>
       </c>
@@ -6493,7 +6492,7 @@
       <c r="W40" s="91"/>
       <c r="X40" s="91"/>
     </row>
-    <row r="41" spans="1:24" s="8" customFormat="1">
+    <row r="41" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>157</v>
       </c>
@@ -6539,7 +6538,7 @@
       <c r="W41" s="91"/>
       <c r="X41" s="91"/>
     </row>
-    <row r="42" spans="1:24" s="8" customFormat="1">
+    <row r="42" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>163</v>
       </c>
@@ -6591,7 +6590,7 @@
       <c r="W42" s="91"/>
       <c r="X42" s="91"/>
     </row>
-    <row r="43" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="43" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>157</v>
       </c>
@@ -6639,7 +6638,7 @@
       <c r="W43" s="91"/>
       <c r="X43" s="91"/>
     </row>
-    <row r="44" spans="1:24" s="8" customFormat="1">
+    <row r="44" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>172</v>
       </c>
@@ -6689,7 +6688,7 @@
       <c r="W44" s="91"/>
       <c r="X44" s="91"/>
     </row>
-    <row r="45" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="45" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>172</v>
       </c>
@@ -6741,7 +6740,7 @@
       <c r="W45" s="91"/>
       <c r="X45" s="91"/>
     </row>
-    <row r="46" spans="1:24" s="8" customFormat="1">
+    <row r="46" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>181</v>
       </c>
@@ -6787,7 +6786,7 @@
       <c r="W46" s="91"/>
       <c r="X46" s="91"/>
     </row>
-    <row r="47" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="47" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>184</v>
       </c>
@@ -6839,7 +6838,7 @@
       <c r="W47" s="91"/>
       <c r="X47" s="91"/>
     </row>
-    <row r="48" spans="1:24" s="8" customFormat="1">
+    <row r="48" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>190</v>
       </c>
@@ -6889,7 +6888,7 @@
       <c r="W48" s="91"/>
       <c r="X48" s="91"/>
     </row>
-    <row r="49" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="49" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>68</v>
       </c>
@@ -6939,7 +6938,7 @@
       <c r="W49" s="91"/>
       <c r="X49" s="91"/>
     </row>
-    <row r="50" spans="1:24" s="8" customFormat="1" ht="24" customHeight="1">
+    <row r="50" spans="1:24" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>208</v>
       </c>
@@ -6991,7 +6990,7 @@
       <c r="W50" s="91"/>
       <c r="X50" s="91"/>
     </row>
-    <row r="51" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="51" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>68</v>
       </c>
@@ -7043,7 +7042,7 @@
       <c r="W51" s="91"/>
       <c r="X51" s="91"/>
     </row>
-    <row r="52" spans="1:24" s="8" customFormat="1" ht="30">
+    <row r="52" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>194</v>
       </c>
@@ -7095,7 +7094,7 @@
       <c r="W52" s="91"/>
       <c r="X52" s="91"/>
     </row>
-    <row r="53" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="53" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>194</v>
       </c>
@@ -7147,7 +7146,7 @@
       <c r="W53" s="91"/>
       <c r="X53" s="91"/>
     </row>
-    <row r="54" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="54" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>51</v>
       </c>
@@ -7199,7 +7198,7 @@
       <c r="W54" s="91"/>
       <c r="X54" s="91"/>
     </row>
-    <row r="55" spans="1:24" s="8" customFormat="1">
+    <row r="55" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>66</v>
       </c>
@@ -7249,7 +7248,7 @@
       <c r="W55" s="91"/>
       <c r="X55" s="91"/>
     </row>
-    <row r="56" spans="1:24" s="8" customFormat="1">
+    <row r="56" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>222</v>
       </c>
@@ -7295,7 +7294,7 @@
       <c r="W56" s="91"/>
       <c r="X56" s="91"/>
     </row>
-    <row r="57" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="57" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>194</v>
       </c>
@@ -7347,7 +7346,7 @@
       <c r="W57" s="91"/>
       <c r="X57" s="91"/>
     </row>
-    <row r="58" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="58" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A58" s="58" t="s">
         <v>194</v>
       </c>
@@ -7397,7 +7396,7 @@
       <c r="W58" s="91"/>
       <c r="X58" s="91"/>
     </row>
-    <row r="59" spans="1:24" s="8" customFormat="1">
+    <row r="59" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="58" t="s">
         <v>194</v>
       </c>
@@ -7449,7 +7448,7 @@
       <c r="W59" s="91"/>
       <c r="X59" s="91"/>
     </row>
-    <row r="60" spans="1:24" s="8" customFormat="1">
+    <row r="60" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="58" t="s">
         <v>194</v>
       </c>
@@ -7501,7 +7500,7 @@
       <c r="W60" s="91"/>
       <c r="X60" s="91"/>
     </row>
-    <row r="61" spans="1:24" s="8" customFormat="1">
+    <row r="61" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="58" t="s">
         <v>235</v>
       </c>
@@ -7553,7 +7552,7 @@
       <c r="W61" s="91"/>
       <c r="X61" s="91"/>
     </row>
-    <row r="62" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="62" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A62" s="58" t="s">
         <v>241</v>
       </c>
@@ -7603,7 +7602,7 @@
       <c r="W62" s="91"/>
       <c r="X62" s="91"/>
     </row>
-    <row r="63" spans="1:24" s="8" customFormat="1">
+    <row r="63" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="58" t="s">
         <v>245</v>
       </c>
@@ -7653,7 +7652,7 @@
       <c r="W63" s="91"/>
       <c r="X63" s="91"/>
     </row>
-    <row r="64" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="64" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A64" s="58" t="s">
         <v>249</v>
       </c>
@@ -7705,7 +7704,7 @@
       <c r="W64" s="91"/>
       <c r="X64" s="91"/>
     </row>
-    <row r="65" spans="1:24" s="8" customFormat="1">
+    <row r="65" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="58" t="s">
         <v>249</v>
       </c>
@@ -7757,7 +7756,7 @@
       <c r="W65" s="91"/>
       <c r="X65" s="91"/>
     </row>
-    <row r="66" spans="1:24" s="8" customFormat="1">
+    <row r="66" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="58" t="s">
         <v>258</v>
       </c>
@@ -7809,7 +7808,7 @@
       <c r="W66" s="91"/>
       <c r="X66" s="91"/>
     </row>
-    <row r="67" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="67" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A67" s="58" t="s">
         <v>245</v>
       </c>
@@ -7859,7 +7858,7 @@
       <c r="W67" s="91"/>
       <c r="X67" s="91"/>
     </row>
-    <row r="68" spans="1:24" s="8" customFormat="1">
+    <row r="68" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="58" t="s">
         <v>245</v>
       </c>
@@ -7909,7 +7908,7 @@
       <c r="W68" s="91"/>
       <c r="X68" s="91"/>
     </row>
-    <row r="69" spans="1:24" s="8" customFormat="1">
+    <row r="69" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="58" t="s">
         <v>245</v>
       </c>
@@ -7957,7 +7956,7 @@
       <c r="W69" s="91"/>
       <c r="X69" s="91"/>
     </row>
-    <row r="70" spans="1:24" s="8" customFormat="1">
+    <row r="70" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="58" t="s">
         <v>273</v>
       </c>
@@ -8009,7 +8008,7 @@
       <c r="W70" s="91"/>
       <c r="X70" s="91"/>
     </row>
-    <row r="71" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="71" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A71" s="58" t="s">
         <v>249</v>
       </c>
@@ -8059,7 +8058,7 @@
       <c r="W71" s="91"/>
       <c r="X71" s="91"/>
     </row>
-    <row r="72" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="72" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A72" s="58" t="s">
         <v>281</v>
       </c>
@@ -8111,7 +8110,7 @@
       <c r="W72" s="91"/>
       <c r="X72" s="91"/>
     </row>
-    <row r="73" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="73" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A73" s="58" t="s">
         <v>108</v>
       </c>
@@ -8161,7 +8160,7 @@
       <c r="W73" s="91"/>
       <c r="X73" s="91"/>
     </row>
-    <row r="74" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="74" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A74" s="58" t="s">
         <v>292</v>
       </c>
@@ -8213,7 +8212,7 @@
       <c r="W74" s="91"/>
       <c r="X74" s="91"/>
     </row>
-    <row r="75" spans="1:24" s="8" customFormat="1">
+    <row r="75" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="58" t="s">
         <v>172</v>
       </c>
@@ -8263,7 +8262,7 @@
       <c r="W75" s="91"/>
       <c r="X75" s="91"/>
     </row>
-    <row r="76" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="76" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A76" s="58" t="s">
         <v>48</v>
       </c>
@@ -8315,7 +8314,7 @@
       <c r="W76" s="91"/>
       <c r="X76" s="91"/>
     </row>
-    <row r="77" spans="1:24" s="8" customFormat="1">
+    <row r="77" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="58" t="s">
         <v>48</v>
       </c>
@@ -8367,7 +8366,7 @@
       <c r="W77" s="91"/>
       <c r="X77" s="91"/>
     </row>
-    <row r="78" spans="1:24" s="8" customFormat="1">
+    <row r="78" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="58" t="s">
         <v>48</v>
       </c>
@@ -8419,7 +8418,7 @@
       <c r="W78" s="91"/>
       <c r="X78" s="91"/>
     </row>
-    <row r="79" spans="1:24" s="8" customFormat="1" ht="30">
+    <row r="79" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="58" t="s">
         <v>309</v>
       </c>
@@ -8471,7 +8470,7 @@
       <c r="W79" s="91"/>
       <c r="X79" s="91"/>
     </row>
-    <row r="80" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="80" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A80" s="58" t="s">
         <v>315</v>
       </c>
@@ -8521,7 +8520,7 @@
       <c r="W80" s="91"/>
       <c r="X80" s="91"/>
     </row>
-    <row r="81" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="81" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A81" s="58" t="s">
         <v>315</v>
       </c>
@@ -8571,7 +8570,7 @@
       <c r="W81" s="91"/>
       <c r="X81" s="91"/>
     </row>
-    <row r="82" spans="1:24" s="8" customFormat="1" ht="40.5">
+    <row r="82" spans="1:24" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A82" s="58" t="s">
         <v>81</v>
       </c>
@@ -8627,7 +8626,7 @@
       <c r="W82" s="91"/>
       <c r="X82" s="91"/>
     </row>
-    <row r="83" spans="1:24" s="8" customFormat="1">
+    <row r="83" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="58" t="s">
         <v>326</v>
       </c>
@@ -8677,7 +8676,7 @@
       <c r="W83" s="91"/>
       <c r="X83" s="91"/>
     </row>
-    <row r="84" spans="1:24" s="8" customFormat="1">
+    <row r="84" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="58" t="s">
         <v>50</v>
       </c>
@@ -8727,7 +8726,7 @@
       <c r="W84" s="91"/>
       <c r="X84" s="91"/>
     </row>
-    <row r="85" spans="1:24" s="8" customFormat="1">
+    <row r="85" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>50</v>
       </c>
@@ -8777,7 +8776,7 @@
       <c r="W85" s="91"/>
       <c r="X85" s="91"/>
     </row>
-    <row r="86" spans="1:24" s="8" customFormat="1">
+    <row r="86" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>336</v>
       </c>
@@ -8825,7 +8824,7 @@
       <c r="W86" s="91"/>
       <c r="X86" s="91"/>
     </row>
-    <row r="87" spans="1:24" s="8" customFormat="1">
+    <row r="87" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>190</v>
       </c>
@@ -8873,7 +8872,7 @@
       <c r="W87" s="91"/>
       <c r="X87" s="91"/>
     </row>
-    <row r="88" spans="1:24" s="8" customFormat="1">
+    <row r="88" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="58" t="s">
         <v>51</v>
       </c>
@@ -8923,7 +8922,7 @@
       <c r="W88" s="91"/>
       <c r="X88" s="91"/>
     </row>
-    <row r="89" spans="1:24" s="8" customFormat="1">
+    <row r="89" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="58" t="s">
         <v>51</v>
       </c>
@@ -8973,7 +8972,7 @@
       <c r="W89" s="91"/>
       <c r="X89" s="91"/>
     </row>
-    <row r="90" spans="1:24" s="8" customFormat="1">
+    <row r="90" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="58" t="s">
         <v>51</v>
       </c>
@@ -9025,7 +9024,7 @@
       <c r="W90" s="91"/>
       <c r="X90" s="91"/>
     </row>
-    <row r="91" spans="1:24" s="8" customFormat="1" ht="30">
+    <row r="91" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="58" t="s">
         <v>51</v>
       </c>
@@ -9075,7 +9074,7 @@
       <c r="W91" s="91"/>
       <c r="X91" s="91"/>
     </row>
-    <row r="92" spans="1:24" s="8" customFormat="1">
+    <row r="92" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="58" t="s">
         <v>51</v>
       </c>
@@ -9125,7 +9124,7 @@
       <c r="W92" s="91"/>
       <c r="X92" s="91"/>
     </row>
-    <row r="93" spans="1:24" s="8" customFormat="1">
+    <row r="93" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="58" t="s">
         <v>355</v>
       </c>
@@ -9177,7 +9176,7 @@
       <c r="W93" s="91"/>
       <c r="X93" s="91"/>
     </row>
-    <row r="94" spans="1:24" s="8" customFormat="1" ht="24.75" customHeight="1">
+    <row r="94" spans="1:24" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="58" t="s">
         <v>50</v>
       </c>
@@ -9227,7 +9226,7 @@
       <c r="W94" s="91"/>
       <c r="X94" s="91"/>
     </row>
-    <row r="95" spans="1:24" s="8" customFormat="1">
+    <row r="95" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="58" t="s">
         <v>52</v>
       </c>
@@ -9277,7 +9276,7 @@
       <c r="W95" s="91"/>
       <c r="X95" s="91"/>
     </row>
-    <row r="96" spans="1:24" s="8" customFormat="1">
+    <row r="96" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="58" t="s">
         <v>52</v>
       </c>
@@ -9327,7 +9326,7 @@
       <c r="W96" s="91"/>
       <c r="X96" s="91"/>
     </row>
-    <row r="97" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="97" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A97" s="79" t="s">
         <v>108</v>
       </c>
@@ -9379,7 +9378,7 @@
       <c r="W97" s="91"/>
       <c r="X97" s="91"/>
     </row>
-    <row r="98" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="98" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A98" s="58" t="s">
         <v>108</v>
       </c>
@@ -9441,7 +9440,7 @@
       <c r="W98" s="91"/>
       <c r="X98" s="91"/>
     </row>
-    <row r="99" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="99" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A99" s="58" t="s">
         <v>27</v>
       </c>
@@ -9493,7 +9492,7 @@
       <c r="W99" s="91"/>
       <c r="X99" s="91"/>
     </row>
-    <row r="100" spans="1:24" s="8" customFormat="1">
+    <row r="100" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="58" t="s">
         <v>48</v>
       </c>
@@ -9545,7 +9544,7 @@
       <c r="W100" s="91"/>
       <c r="X100" s="91"/>
     </row>
-    <row r="101" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="101" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A101" s="58" t="s">
         <v>38</v>
       </c>
@@ -9597,7 +9596,7 @@
       <c r="W101" s="91"/>
       <c r="X101" s="91"/>
     </row>
-    <row r="102" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="102" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A102" s="58" t="s">
         <v>108</v>
       </c>
@@ -9647,7 +9646,7 @@
       <c r="W102" s="91"/>
       <c r="X102" s="91"/>
     </row>
-    <row r="103" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="103" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A103" s="58" t="s">
         <v>108</v>
       </c>
@@ -9697,7 +9696,7 @@
       <c r="W103" s="91"/>
       <c r="X103" s="91"/>
     </row>
-    <row r="104" spans="1:24" s="8" customFormat="1">
+    <row r="104" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="58" t="s">
         <v>46</v>
       </c>
@@ -9747,7 +9746,7 @@
       <c r="W104" s="91"/>
       <c r="X104" s="91"/>
     </row>
-    <row r="105" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="105" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A105" s="58" t="s">
         <v>108</v>
       </c>
@@ -9797,7 +9796,7 @@
       <c r="W105" s="91"/>
       <c r="X105" s="91"/>
     </row>
-    <row r="106" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="106" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A106" s="58" t="s">
         <v>51</v>
       </c>
@@ -9849,7 +9848,7 @@
       <c r="W106" s="91"/>
       <c r="X106" s="91"/>
     </row>
-    <row r="107" spans="1:24" s="8" customFormat="1">
+    <row r="107" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="58" t="s">
         <v>51</v>
       </c>
@@ -9901,7 +9900,7 @@
       <c r="W107" s="91"/>
       <c r="X107" s="91"/>
     </row>
-    <row r="108" spans="1:24" s="8" customFormat="1">
+    <row r="108" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="58" t="s">
         <v>27</v>
       </c>
@@ -9955,7 +9954,7 @@
       <c r="W108" s="91"/>
       <c r="X108" s="91"/>
     </row>
-    <row r="109" spans="1:24" s="8" customFormat="1">
+    <row r="109" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="58" t="s">
         <v>48</v>
       </c>
@@ -10007,7 +10006,7 @@
       <c r="W109" s="91"/>
       <c r="X109" s="91"/>
     </row>
-    <row r="110" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="110" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A110" s="58" t="s">
         <v>51</v>
       </c>
@@ -10057,7 +10056,7 @@
       <c r="W110" s="91"/>
       <c r="X110" s="91"/>
     </row>
-    <row r="111" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="111" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A111" s="58" t="s">
         <v>405</v>
       </c>
@@ -10105,7 +10104,7 @@
       <c r="W111" s="91"/>
       <c r="X111" s="91"/>
     </row>
-    <row r="112" spans="1:24" s="8" customFormat="1">
+    <row r="112" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="58" t="s">
         <v>52</v>
       </c>
@@ -10157,7 +10156,7 @@
       <c r="W112" s="91"/>
       <c r="X112" s="91"/>
     </row>
-    <row r="113" spans="1:24" s="8" customFormat="1">
+    <row r="113" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="58" t="s">
         <v>51</v>
       </c>
@@ -10207,7 +10206,7 @@
       <c r="W113" s="91"/>
       <c r="X113" s="91"/>
     </row>
-    <row r="114" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="114" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A114" s="58" t="s">
         <v>412</v>
       </c>
@@ -10259,7 +10258,7 @@
       <c r="W114" s="91"/>
       <c r="X114" s="91"/>
     </row>
-    <row r="115" spans="1:24" s="8" customFormat="1">
+    <row r="115" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="58" t="s">
         <v>48</v>
       </c>
@@ -10309,7 +10308,7 @@
       <c r="W115" s="91"/>
       <c r="X115" s="91"/>
     </row>
-    <row r="116" spans="1:24" s="8" customFormat="1">
+    <row r="116" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="58" t="s">
         <v>235</v>
       </c>
@@ -10359,7 +10358,7 @@
       <c r="W116" s="91"/>
       <c r="X116" s="91"/>
     </row>
-    <row r="117" spans="1:24" s="8" customFormat="1">
+    <row r="117" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="58" t="s">
         <v>50</v>
       </c>
@@ -10409,7 +10408,7 @@
       <c r="W117" s="91"/>
       <c r="X117" s="91"/>
     </row>
-    <row r="118" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="118" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A118" s="58" t="s">
         <v>427</v>
       </c>
@@ -10457,7 +10456,7 @@
       <c r="W118" s="91"/>
       <c r="X118" s="91"/>
     </row>
-    <row r="119" spans="1:24" s="8" customFormat="1">
+    <row r="119" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="58" t="s">
         <v>54</v>
       </c>
@@ -10509,7 +10508,7 @@
       <c r="W119" s="91"/>
       <c r="X119" s="91"/>
     </row>
-    <row r="120" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="120" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A120" s="58" t="s">
         <v>38</v>
       </c>
@@ -10561,7 +10560,7 @@
       <c r="W120" s="91"/>
       <c r="X120" s="91"/>
     </row>
-    <row r="121" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="121" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A121" s="58" t="s">
         <v>38</v>
       </c>
@@ -10613,7 +10612,7 @@
       <c r="W121" s="91"/>
       <c r="X121" s="91"/>
     </row>
-    <row r="122" spans="1:24" s="8" customFormat="1">
+    <row r="122" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="58" t="s">
         <v>54</v>
       </c>
@@ -10663,7 +10662,7 @@
       <c r="W122" s="91"/>
       <c r="X122" s="91"/>
     </row>
-    <row r="123" spans="1:24" s="8" customFormat="1" ht="27.75" customHeight="1">
+    <row r="123" spans="1:24" s="8" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="58" t="s">
         <v>446</v>
       </c>
@@ -10711,7 +10710,7 @@
       <c r="W123" s="91"/>
       <c r="X123" s="91"/>
     </row>
-    <row r="124" spans="1:24" s="8" customFormat="1" ht="40.5">
+    <row r="124" spans="1:24" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A124" s="58" t="s">
         <v>450</v>
       </c>
@@ -10763,7 +10762,7 @@
       <c r="W124" s="91"/>
       <c r="X124" s="91"/>
     </row>
-    <row r="125" spans="1:24" s="8" customFormat="1">
+    <row r="125" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="58" t="s">
         <v>54</v>
       </c>
@@ -10815,7 +10814,7 @@
       <c r="W125" s="91"/>
       <c r="X125" s="91"/>
     </row>
-    <row r="126" spans="1:24" s="8" customFormat="1">
+    <row r="126" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="58" t="s">
         <v>52</v>
       </c>
@@ -10867,7 +10866,7 @@
       <c r="W126" s="91"/>
       <c r="X126" s="91"/>
     </row>
-    <row r="127" spans="1:24" s="8" customFormat="1">
+    <row r="127" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="58" t="s">
         <v>54</v>
       </c>
@@ -10919,7 +10918,7 @@
       <c r="W127" s="91"/>
       <c r="X127" s="91"/>
     </row>
-    <row r="128" spans="1:24" s="8" customFormat="1">
+    <row r="128" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="58" t="s">
         <v>52</v>
       </c>
@@ -10971,7 +10970,7 @@
       <c r="W128" s="91"/>
       <c r="X128" s="91"/>
     </row>
-    <row r="129" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="129" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A129" s="58" t="s">
         <v>464</v>
       </c>
@@ -11021,7 +11020,7 @@
       <c r="W129" s="91"/>
       <c r="X129" s="91"/>
     </row>
-    <row r="130" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="130" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A130" s="58" t="s">
         <v>51</v>
       </c>
@@ -11071,7 +11070,7 @@
       <c r="W130" s="91"/>
       <c r="X130" s="91"/>
     </row>
-    <row r="131" spans="1:24" s="8" customFormat="1">
+    <row r="131" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="58" t="s">
         <v>222</v>
       </c>
@@ -11121,7 +11120,7 @@
       <c r="W131" s="91"/>
       <c r="X131" s="91"/>
     </row>
-    <row r="132" spans="1:24" s="8" customFormat="1">
+    <row r="132" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="58" t="s">
         <v>27</v>
       </c>
@@ -11173,7 +11172,7 @@
       <c r="W132" s="91"/>
       <c r="X132" s="91"/>
     </row>
-    <row r="133" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="133" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A133" s="58" t="s">
         <v>108</v>
       </c>
@@ -11225,7 +11224,7 @@
       <c r="W133" s="91"/>
       <c r="X133" s="91"/>
     </row>
-    <row r="134" spans="1:24" s="8" customFormat="1">
+    <row r="134" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="58" t="s">
         <v>45</v>
       </c>
@@ -11273,7 +11272,7 @@
       <c r="W134" s="91"/>
       <c r="X134" s="91"/>
     </row>
-    <row r="135" spans="1:24" s="8" customFormat="1">
+    <row r="135" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="58" t="s">
         <v>27</v>
       </c>
@@ -11323,7 +11322,7 @@
       <c r="W135" s="91"/>
       <c r="X135" s="91"/>
     </row>
-    <row r="136" spans="1:24" s="8" customFormat="1">
+    <row r="136" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>52</v>
       </c>
@@ -11373,7 +11372,7 @@
       <c r="W136" s="91"/>
       <c r="X136" s="91"/>
     </row>
-    <row r="137" spans="1:24" s="8" customFormat="1">
+    <row r="137" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>51</v>
       </c>
@@ -11423,7 +11422,7 @@
       <c r="W137" s="91"/>
       <c r="X137" s="91"/>
     </row>
-    <row r="138" spans="1:24" s="8" customFormat="1">
+    <row r="138" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>51</v>
       </c>
@@ -11473,7 +11472,7 @@
       <c r="W138" s="91"/>
       <c r="X138" s="91"/>
     </row>
-    <row r="139" spans="1:24" s="8" customFormat="1">
+    <row r="139" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>48</v>
       </c>
@@ -11525,7 +11524,7 @@
       <c r="W139" s="91"/>
       <c r="X139" s="91"/>
     </row>
-    <row r="140" spans="1:24" s="8" customFormat="1">
+    <row r="140" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>52</v>
       </c>
@@ -11575,7 +11574,7 @@
       <c r="W140" s="91"/>
       <c r="X140" s="91"/>
     </row>
-    <row r="141" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="141" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>38</v>
       </c>
@@ -11625,7 +11624,7 @@
       <c r="W141" s="91"/>
       <c r="X141" s="91"/>
     </row>
-    <row r="142" spans="1:24" s="8" customFormat="1" ht="30">
+    <row r="142" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>38</v>
       </c>
@@ -11677,7 +11676,7 @@
       <c r="W142" s="91"/>
       <c r="X142" s="91"/>
     </row>
-    <row r="143" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="143" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>38</v>
       </c>
@@ -11727,7 +11726,7 @@
       <c r="W143" s="91"/>
       <c r="X143" s="91"/>
     </row>
-    <row r="144" spans="1:24" s="8" customFormat="1">
+    <row r="144" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>38</v>
       </c>
@@ -11777,7 +11776,7 @@
       <c r="W144" s="91"/>
       <c r="X144" s="91"/>
     </row>
-    <row r="145" spans="1:24" s="8" customFormat="1">
+    <row r="145" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>54</v>
       </c>
@@ -11827,7 +11826,7 @@
       <c r="W145" s="91"/>
       <c r="X145" s="91"/>
     </row>
-    <row r="146" spans="1:24" s="8" customFormat="1">
+    <row r="146" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>54</v>
       </c>
@@ -11877,7 +11876,7 @@
       <c r="W146" s="91"/>
       <c r="X146" s="91"/>
     </row>
-    <row r="147" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="147" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>46</v>
       </c>
@@ -11927,7 +11926,7 @@
       <c r="W147" s="91"/>
       <c r="X147" s="91"/>
     </row>
-    <row r="148" spans="1:24" s="8" customFormat="1">
+    <row r="148" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>27</v>
       </c>
@@ -11977,7 +11976,7 @@
       <c r="W148" s="91"/>
       <c r="X148" s="91"/>
     </row>
-    <row r="149" spans="1:24" s="8" customFormat="1">
+    <row r="149" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>45</v>
       </c>
@@ -12029,7 +12028,7 @@
       <c r="W149" s="91"/>
       <c r="X149" s="91"/>
     </row>
-    <row r="150" spans="1:24" s="8" customFormat="1">
+    <row r="150" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>45</v>
       </c>
@@ -12081,7 +12080,7 @@
       <c r="W150" s="91"/>
       <c r="X150" s="91"/>
     </row>
-    <row r="151" spans="1:24" s="8" customFormat="1">
+    <row r="151" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>427</v>
       </c>
@@ -12131,7 +12130,7 @@
       <c r="W151" s="91"/>
       <c r="X151" s="91"/>
     </row>
-    <row r="152" spans="1:24" s="8" customFormat="1">
+    <row r="152" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>51</v>
       </c>
@@ -12181,7 +12180,7 @@
       <c r="W152" s="91"/>
       <c r="X152" s="91"/>
     </row>
-    <row r="153" spans="1:24" s="8" customFormat="1" ht="40.5">
+    <row r="153" spans="1:24" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>57</v>
       </c>
@@ -12231,7 +12230,7 @@
       <c r="W153" s="91"/>
       <c r="X153" s="91"/>
     </row>
-    <row r="154" spans="1:24" s="8" customFormat="1" ht="40.5">
+    <row r="154" spans="1:24" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>57</v>
       </c>
@@ -12281,7 +12280,7 @@
       <c r="W154" s="91"/>
       <c r="X154" s="91"/>
     </row>
-    <row r="155" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="155" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A155" s="58" t="s">
         <v>57</v>
       </c>
@@ -12329,7 +12328,7 @@
       <c r="W155" s="91"/>
       <c r="X155" s="91"/>
     </row>
-    <row r="156" spans="1:24" s="8" customFormat="1">
+    <row r="156" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="58" t="s">
         <v>54</v>
       </c>
@@ -12379,7 +12378,7 @@
       <c r="W156" s="91"/>
       <c r="X156" s="91"/>
     </row>
-    <row r="157" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="157" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
         <v>51</v>
       </c>
@@ -12429,7 +12428,7 @@
       <c r="W157" s="91"/>
       <c r="X157" s="91"/>
     </row>
-    <row r="158" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="158" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A158" s="58" t="s">
         <v>532</v>
       </c>
@@ -12479,7 +12478,7 @@
       <c r="W158" s="91"/>
       <c r="X158" s="91"/>
     </row>
-    <row r="159" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="159" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A159" s="58" t="s">
         <v>52</v>
       </c>
@@ -12531,7 +12530,7 @@
       <c r="W159" s="91"/>
       <c r="X159" s="91"/>
     </row>
-    <row r="160" spans="1:24" s="8" customFormat="1">
+    <row r="160" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="58" t="s">
         <v>48</v>
       </c>
@@ -12581,7 +12580,7 @@
       <c r="W160" s="91"/>
       <c r="X160" s="91"/>
     </row>
-    <row r="161" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="161" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A161" s="58" t="s">
         <v>538</v>
       </c>
@@ -12631,7 +12630,7 @@
       <c r="W161" s="91"/>
       <c r="X161" s="91"/>
     </row>
-    <row r="162" spans="1:24" s="8" customFormat="1">
+    <row r="162" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="58" t="s">
         <v>27</v>
       </c>
@@ -12687,7 +12686,7 @@
       <c r="W162" s="91"/>
       <c r="X162" s="91"/>
     </row>
-    <row r="163" spans="1:24" s="8" customFormat="1">
+    <row r="163" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>50</v>
       </c>
@@ -12729,7 +12728,7 @@
       <c r="W163" s="91"/>
       <c r="X163" s="91"/>
     </row>
-    <row r="164" spans="1:24" s="8" customFormat="1">
+    <row r="164" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>53</v>
       </c>
@@ -12771,7 +12770,7 @@
       <c r="W164" s="91"/>
       <c r="X164" s="91"/>
     </row>
-    <row r="165" spans="1:24" s="8" customFormat="1">
+    <row r="165" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="58" t="s">
         <v>545</v>
       </c>
@@ -12823,7 +12822,7 @@
       <c r="W165" s="91"/>
       <c r="X165" s="91"/>
     </row>
-    <row r="166" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="166" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A166" s="58" t="s">
         <v>551</v>
       </c>
@@ -12875,7 +12874,7 @@
       <c r="W166" s="91"/>
       <c r="X166" s="91"/>
     </row>
-    <row r="167" spans="1:24" s="8" customFormat="1">
+    <row r="167" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="58" t="s">
         <v>54</v>
       </c>
@@ -12929,7 +12928,7 @@
       <c r="W167" s="91"/>
       <c r="X167" s="91"/>
     </row>
-    <row r="168" spans="1:24" s="8" customFormat="1">
+    <row r="168" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="58" t="s">
         <v>172</v>
       </c>
@@ -12981,7 +12980,7 @@
       <c r="W168" s="91"/>
       <c r="X168" s="91"/>
     </row>
-    <row r="169" spans="1:24" s="8" customFormat="1">
+    <row r="169" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="58" t="s">
         <v>46</v>
       </c>
@@ -13033,7 +13032,7 @@
       <c r="W169" s="91"/>
       <c r="X169" s="91"/>
     </row>
-    <row r="170" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="170" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A170" s="58" t="s">
         <v>72</v>
       </c>
@@ -13083,7 +13082,7 @@
       <c r="W170" s="91"/>
       <c r="X170" s="91"/>
     </row>
-    <row r="171" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="171" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A171" s="58" t="s">
         <v>72</v>
       </c>
@@ -13133,7 +13132,7 @@
       <c r="W171" s="91"/>
       <c r="X171" s="91"/>
     </row>
-    <row r="172" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="172" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A172" s="58" t="s">
         <v>72</v>
       </c>
@@ -13183,7 +13182,7 @@
       <c r="W172" s="91"/>
       <c r="X172" s="91"/>
     </row>
-    <row r="173" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="173" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A173" s="58" t="s">
         <v>72</v>
       </c>
@@ -13233,7 +13232,7 @@
       <c r="W173" s="91"/>
       <c r="X173" s="91"/>
     </row>
-    <row r="174" spans="1:24" s="8" customFormat="1">
+    <row r="174" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="6"/>
@@ -13261,7 +13260,7 @@
       <c r="W174" s="91"/>
       <c r="X174" s="91"/>
     </row>
-    <row r="175" spans="1:24" s="8" customFormat="1">
+    <row r="175" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="58" t="s">
         <v>46</v>
       </c>
@@ -13313,7 +13312,7 @@
       <c r="W175" s="91"/>
       <c r="X175" s="91"/>
     </row>
-    <row r="176" spans="1:24" s="8" customFormat="1">
+    <row r="176" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="58" t="s">
         <v>46</v>
       </c>
@@ -13365,7 +13364,7 @@
       <c r="W176" s="91"/>
       <c r="X176" s="91"/>
     </row>
-    <row r="177" spans="1:24" s="8" customFormat="1">
+    <row r="177" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="58" t="s">
         <v>46</v>
       </c>
@@ -13417,7 +13416,7 @@
       <c r="W177" s="91"/>
       <c r="X177" s="91"/>
     </row>
-    <row r="178" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="178" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A178" s="58" t="s">
         <v>46</v>
       </c>
@@ -13467,7 +13466,7 @@
       <c r="W178" s="91"/>
       <c r="X178" s="91"/>
     </row>
-    <row r="179" spans="1:24" s="8" customFormat="1">
+    <row r="179" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="58" t="s">
         <v>46</v>
       </c>
@@ -13517,7 +13516,7 @@
       <c r="W179" s="91"/>
       <c r="X179" s="91"/>
     </row>
-    <row r="180" spans="1:24" s="8" customFormat="1">
+    <row r="180" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="58" t="s">
         <v>46</v>
       </c>
@@ -13569,7 +13568,7 @@
       <c r="W180" s="91"/>
       <c r="X180" s="91"/>
     </row>
-    <row r="181" spans="1:24" s="8" customFormat="1">
+    <row r="181" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="58" t="s">
         <v>46</v>
       </c>
@@ -13619,7 +13618,7 @@
       <c r="W181" s="91"/>
       <c r="X181" s="91"/>
     </row>
-    <row r="182" spans="1:24" s="8" customFormat="1">
+    <row r="182" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="58" t="s">
         <v>46</v>
       </c>
@@ -13671,7 +13670,7 @@
       <c r="W182" s="91"/>
       <c r="X182" s="91"/>
     </row>
-    <row r="183" spans="1:24" s="8" customFormat="1">
+    <row r="183" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="58" t="s">
         <v>46</v>
       </c>
@@ -13723,7 +13722,7 @@
       <c r="W183" s="91"/>
       <c r="X183" s="91"/>
     </row>
-    <row r="184" spans="1:24" s="8" customFormat="1">
+    <row r="184" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="58" t="s">
         <v>46</v>
       </c>
@@ -13771,7 +13770,7 @@
       <c r="W184" s="91"/>
       <c r="X184" s="91"/>
     </row>
-    <row r="185" spans="1:24" s="8" customFormat="1">
+    <row r="185" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="58" t="s">
         <v>46</v>
       </c>
@@ -13823,7 +13822,7 @@
       <c r="W185" s="91"/>
       <c r="X185" s="91"/>
     </row>
-    <row r="186" spans="1:24" s="8" customFormat="1">
+    <row r="186" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="58" t="s">
         <v>46</v>
       </c>
@@ -13873,7 +13872,7 @@
       <c r="W186" s="91"/>
       <c r="X186" s="91"/>
     </row>
-    <row r="187" spans="1:24" s="8" customFormat="1">
+    <row r="187" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="58" t="s">
         <v>46</v>
       </c>
@@ -13925,7 +13924,7 @@
       <c r="W187" s="91"/>
       <c r="X187" s="91"/>
     </row>
-    <row r="188" spans="1:24" s="8" customFormat="1">
+    <row r="188" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="58" t="s">
         <v>46</v>
       </c>
@@ -13977,7 +13976,7 @@
       <c r="W188" s="91"/>
       <c r="X188" s="91"/>
     </row>
-    <row r="189" spans="1:24" s="8" customFormat="1">
+    <row r="189" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="58" t="s">
         <v>46</v>
       </c>
@@ -14029,7 +14028,7 @@
       <c r="W189" s="91"/>
       <c r="X189" s="91"/>
     </row>
-    <row r="190" spans="1:24" s="8" customFormat="1">
+    <row r="190" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="58" t="s">
         <v>46</v>
       </c>
@@ -14079,7 +14078,7 @@
       <c r="W190" s="91"/>
       <c r="X190" s="91"/>
     </row>
-    <row r="191" spans="1:24" s="8" customFormat="1">
+    <row r="191" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="58" t="s">
         <v>46</v>
       </c>
@@ -14131,7 +14130,7 @@
       <c r="W191" s="91"/>
       <c r="X191" s="91"/>
     </row>
-    <row r="192" spans="1:24" s="8" customFormat="1">
+    <row r="192" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="58" t="s">
         <v>46</v>
       </c>
@@ -14183,7 +14182,7 @@
       <c r="W192" s="91"/>
       <c r="X192" s="91"/>
     </row>
-    <row r="193" spans="1:24" s="8" customFormat="1">
+    <row r="193" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="58" t="s">
         <v>46</v>
       </c>
@@ -14233,7 +14232,7 @@
       <c r="W193" s="91"/>
       <c r="X193" s="91"/>
     </row>
-    <row r="194" spans="1:24" s="8" customFormat="1">
+    <row r="194" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="58" t="s">
         <v>46</v>
       </c>
@@ -14285,7 +14284,7 @@
       <c r="W194" s="91"/>
       <c r="X194" s="91"/>
     </row>
-    <row r="195" spans="1:24" s="8" customFormat="1">
+    <row r="195" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="58" t="s">
         <v>46</v>
       </c>
@@ -14337,7 +14336,7 @@
       <c r="W195" s="91"/>
       <c r="X195" s="91"/>
     </row>
-    <row r="196" spans="1:24" s="8" customFormat="1">
+    <row r="196" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="58" t="s">
         <v>46</v>
       </c>
@@ -14389,7 +14388,7 @@
       <c r="W196" s="91"/>
       <c r="X196" s="91"/>
     </row>
-    <row r="197" spans="1:24" s="8" customFormat="1" ht="27">
+    <row r="197" spans="1:24" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A197" s="58" t="s">
         <v>46</v>
       </c>
@@ -14441,7 +14440,7 @@
       <c r="W197" s="91"/>
       <c r="X197" s="91"/>
     </row>
-    <row r="198" spans="1:24" s="8" customFormat="1">
+    <row r="198" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="58" t="s">
         <v>46</v>
       </c>
@@ -14493,7 +14492,7 @@
       <c r="W198" s="91"/>
       <c r="X198" s="91"/>
     </row>
-    <row r="199" spans="1:24" s="8" customFormat="1">
+    <row r="199" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="58"/>
       <c r="B199" s="58"/>
       <c r="C199" s="59"/>
@@ -14519,7 +14518,7 @@
       <c r="W199" s="91"/>
       <c r="X199" s="91"/>
     </row>
-    <row r="200" spans="1:24" s="8" customFormat="1">
+    <row r="200" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="58"/>
       <c r="B200" s="58"/>
       <c r="C200" s="59"/>
@@ -14545,7 +14544,7 @@
       <c r="W200" s="91"/>
       <c r="X200" s="91"/>
     </row>
-    <row r="201" spans="1:24" s="8" customFormat="1">
+    <row r="201" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="58"/>
       <c r="B201" s="58"/>
       <c r="C201" s="59"/>
@@ -14571,7 +14570,7 @@
       <c r="W201" s="91"/>
       <c r="X201" s="91"/>
     </row>
-    <row r="202" spans="1:24" s="8" customFormat="1">
+    <row r="202" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="58"/>
       <c r="B202" s="58"/>
       <c r="C202" s="59"/>
@@ -14597,7 +14596,7 @@
       <c r="W202" s="91"/>
       <c r="X202" s="91"/>
     </row>
-    <row r="203" spans="1:24" s="8" customFormat="1">
+    <row r="203" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="6"/>
@@ -14623,7 +14622,7 @@
       <c r="W203" s="91"/>
       <c r="X203" s="91"/>
     </row>
-    <row r="204" spans="1:24" s="8" customFormat="1">
+    <row r="204" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="6"/>
@@ -14649,7 +14648,7 @@
       <c r="W204" s="91"/>
       <c r="X204" s="91"/>
     </row>
-    <row r="205" spans="1:24" s="8" customFormat="1">
+    <row r="205" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="6"/>
@@ -14675,7 +14674,7 @@
       <c r="W205" s="91"/>
       <c r="X205" s="91"/>
     </row>
-    <row r="206" spans="1:24" s="8" customFormat="1">
+    <row r="206" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="6"/>
@@ -14701,7 +14700,7 @@
       <c r="W206" s="91"/>
       <c r="X206" s="91"/>
     </row>
-    <row r="207" spans="1:24" s="8" customFormat="1">
+    <row r="207" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="16"/>
       <c r="B207" s="16"/>
       <c r="C207" s="17"/>
@@ -14739,7 +14738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -14750,7 +14749,7 @@
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
@@ -14765,7 +14764,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27.75">
+    <row r="1" spans="1:12" ht="27.75" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
         <v>23</v>
       </c>
@@ -14781,13 +14780,13 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L2" s="34"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L3" s="33"/>
     </row>
-    <row r="4" spans="1:12" ht="25.5">
+    <row r="4" spans="1:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A4" s="51" t="s">
         <v>24</v>
       </c>
@@ -14825,7 +14824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -14839,7 +14838,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -14853,7 +14852,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -14867,7 +14866,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -14881,7 +14880,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -14895,7 +14894,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -14909,7 +14908,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -14923,7 +14922,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -14937,7 +14936,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -14951,7 +14950,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -14965,7 +14964,7 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -14979,7 +14978,7 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -14993,7 +14992,7 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -15007,7 +15006,7 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -15021,7 +15020,7 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -15035,7 +15034,7 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -15049,7 +15048,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -15063,7 +15062,7 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -15077,7 +15076,7 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -15091,7 +15090,7 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -15105,7 +15104,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -15119,7 +15118,7 @@
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -15133,7 +15132,7 @@
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -15147,7 +15146,7 @@
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -15161,7 +15160,7 @@
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -15175,7 +15174,7 @@
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -15189,7 +15188,7 @@
       <c r="K30" s="23"/>
       <c r="L30" s="23"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -15203,7 +15202,7 @@
       <c r="K31" s="23"/>
       <c r="L31" s="23"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
@@ -15217,7 +15216,7 @@
       <c r="K32" s="23"/>
       <c r="L32" s="23"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="23"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
@@ -15231,7 +15230,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="23"/>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -15245,7 +15244,7 @@
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="23"/>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -15259,7 +15258,7 @@
       <c r="K35" s="23"/>
       <c r="L35" s="23"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="23"/>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -15273,7 +15272,7 @@
       <c r="K36" s="23"/>
       <c r="L36" s="23"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="23"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -15287,7 +15286,7 @@
       <c r="K37" s="23"/>
       <c r="L37" s="23"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
@@ -15301,7 +15300,7 @@
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
@@ -15327,28 +15326,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="15.75">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -15356,17 +15355,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="16.5">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="11">
         <f ca="1">TODAY()</f>
-        <v>44074</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="6" spans="1:13" s="1" customFormat="1" ht="16.5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="94" t="s">
         <v>9</v>
       </c>
@@ -15387,7 +15386,7 @@
       <c r="L6" s="94"/>
       <c r="M6" s="94"/>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" ht="24.75" customHeight="1">
+    <row r="7" spans="1:13" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>0</v>
       </c>
@@ -15428,7 +15427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1">
+    <row r="8" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="43"/>
       <c r="B8" s="44"/>
       <c r="C8" s="45"/>
@@ -15443,7 +15442,7 @@
       <c r="L8" s="45"/>
       <c r="M8" s="45"/>
     </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1">
+    <row r="9" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43"/>
       <c r="B9" s="44"/>
       <c r="C9" s="45"/>
@@ -15458,7 +15457,7 @@
       <c r="L9" s="45"/>
       <c r="M9" s="45"/>
     </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1">
+    <row r="10" spans="1:13" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
@@ -15473,7 +15472,7 @@
       <c r="L10" s="45"/>
       <c r="M10" s="45"/>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="46"/>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
@@ -15488,7 +15487,7 @@
       <c r="L11" s="46"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46"/>
       <c r="B12" s="46"/>
       <c r="C12" s="46"/>
@@ -15503,7 +15502,7 @@
       <c r="L12" s="46"/>
       <c r="M12" s="46"/>
     </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1">
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46"/>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -15518,7 +15517,7 @@
       <c r="L13" s="46"/>
       <c r="M13" s="46"/>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46"/>
       <c r="B14" s="46"/>
       <c r="C14" s="46"/>
@@ -15533,7 +15532,7 @@
       <c r="L14" s="46"/>
       <c r="M14" s="46"/>
     </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1">
+    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
@@ -15548,7 +15547,7 @@
       <c r="L15" s="46"/>
       <c r="M15" s="46"/>
     </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1">
+    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46"/>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
@@ -15563,7 +15562,7 @@
       <c r="L16" s="46"/>
       <c r="M16" s="46"/>
     </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1">
+    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46"/>
       <c r="B17" s="46"/>
       <c r="C17" s="46"/>
@@ -15578,7 +15577,7 @@
       <c r="L17" s="46"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
+    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
@@ -15593,7 +15592,7 @@
       <c r="L18" s="46"/>
       <c r="M18" s="46"/>
     </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1">
+    <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="46"/>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
@@ -15608,7 +15607,7 @@
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
     </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1">
+    <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="46"/>
       <c r="B20" s="46"/>
       <c r="C20" s="46"/>
@@ -15623,7 +15622,7 @@
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1">
+    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>

</xml_diff>